<commit_message>
Flat - Texture disambiguation
</commit_message>
<xml_diff>
--- a/pk3/FLAT DISAMBIUATOR.xlsx
+++ b/pk3/FLAT DISAMBIUATOR.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="375">
   <si>
     <t>Name</t>
   </si>
@@ -904,6 +904,243 @@
   </si>
   <si>
     <t>ALWAYS</t>
+  </si>
+  <si>
+    <t>C:\Users\TwoIsOne\Desktop\5.22.19\WORKSPACE5\pk3\Flats\2\</t>
+  </si>
+  <si>
+    <t>BRIKGTH1</t>
+  </si>
+  <si>
+    <t>CWMC04</t>
+  </si>
+  <si>
+    <t>CWSNOW2</t>
+  </si>
+  <si>
+    <t>CWSNOW4</t>
+  </si>
+  <si>
+    <t>CWWARN</t>
+  </si>
+  <si>
+    <t>INCDECP1</t>
+  </si>
+  <si>
+    <t>KS_CEM10</t>
+  </si>
+  <si>
+    <t>KS_CEM11</t>
+  </si>
+  <si>
+    <t>KS_CEM14</t>
+  </si>
+  <si>
+    <t>KS_CEM17</t>
+  </si>
+  <si>
+    <t>KS_CEM19</t>
+  </si>
+  <si>
+    <t>KS_CEM20</t>
+  </si>
+  <si>
+    <t>KS_CEM21</t>
+  </si>
+  <si>
+    <t>KS_DIAG1</t>
+  </si>
+  <si>
+    <t>KS_DIAG2</t>
+  </si>
+  <si>
+    <t>LIGHT1</t>
+  </si>
+  <si>
+    <t>LIGHT2</t>
+  </si>
+  <si>
+    <t>LITEB2</t>
+  </si>
+  <si>
+    <t>LITERED2</t>
+  </si>
+  <si>
+    <t>LITEY1</t>
+  </si>
+  <si>
+    <t>METLSL05</t>
+  </si>
+  <si>
+    <t>N_CGRN01</t>
+  </si>
+  <si>
+    <t>N_CGRN02</t>
+  </si>
+  <si>
+    <t>N_CMPGRE</t>
+  </si>
+  <si>
+    <t>QSLIP5</t>
+  </si>
+  <si>
+    <t>STEP00</t>
+  </si>
+  <si>
+    <t>WHPIPEC1</t>
+  </si>
+  <si>
+    <t>WHPIPEC2</t>
+  </si>
+  <si>
+    <t>WHPIPEC3</t>
+  </si>
+  <si>
+    <t>WHPIPEC4</t>
+  </si>
+  <si>
+    <t>FD140</t>
+  </si>
+  <si>
+    <t>FD141</t>
+  </si>
+  <si>
+    <t>FD142</t>
+  </si>
+  <si>
+    <t>FD143</t>
+  </si>
+  <si>
+    <t>FD144</t>
+  </si>
+  <si>
+    <t>FD145</t>
+  </si>
+  <si>
+    <t>FD146</t>
+  </si>
+  <si>
+    <t>FD147</t>
+  </si>
+  <si>
+    <t>FD148</t>
+  </si>
+  <si>
+    <t>FD149</t>
+  </si>
+  <si>
+    <t>FD150</t>
+  </si>
+  <si>
+    <t>FD151</t>
+  </si>
+  <si>
+    <t>FD152</t>
+  </si>
+  <si>
+    <t>FD153</t>
+  </si>
+  <si>
+    <t>FD154</t>
+  </si>
+  <si>
+    <t>FD155</t>
+  </si>
+  <si>
+    <t>FD156</t>
+  </si>
+  <si>
+    <t>FD157</t>
+  </si>
+  <si>
+    <t>FD158</t>
+  </si>
+  <si>
+    <t>FD159</t>
+  </si>
+  <si>
+    <t>FD160</t>
+  </si>
+  <si>
+    <t>FD161</t>
+  </si>
+  <si>
+    <t>FD162</t>
+  </si>
+  <si>
+    <t>FD163</t>
+  </si>
+  <si>
+    <t>FD164</t>
+  </si>
+  <si>
+    <t>FD165</t>
+  </si>
+  <si>
+    <t>FD166</t>
+  </si>
+  <si>
+    <t>FD167</t>
+  </si>
+  <si>
+    <t>FD168</t>
+  </si>
+  <si>
+    <t>FD169</t>
+  </si>
+  <si>
+    <t>Note to self</t>
+  </si>
+  <si>
+    <t>if there are 0 replacements it could be because they have already been replaced in wads. Keep truckin</t>
+  </si>
+  <si>
+    <t>Original flats on the left should be deleted from flats folder</t>
+  </si>
+  <si>
+    <t>That will make sorting and renaming easier, but this list should remain right? Just in cause some old ones need to be disamiguated?</t>
+  </si>
+  <si>
+    <t>Its getting to complicated to handle. Only do this for builds.</t>
+  </si>
+  <si>
+    <t>If the originals are not deleted, it affects nothing in game. If in doubt leave them</t>
+  </si>
+  <si>
+    <t>Do not delete this list that shows the relationship between the old flat names and new flat names.</t>
+  </si>
+  <si>
+    <t>Do delete the flats.</t>
+  </si>
+  <si>
+    <t>Don't do find and replace for the old one's unless you see something in the maps?</t>
+  </si>
+  <si>
+    <t>If someone sees an out of place flat, and it turns out to be a disambiguation problem, run this entire list.</t>
+  </si>
+  <si>
+    <t>If new flats are introduced that replace the old flat names on the left, aren't those all new flats? I'm having trouble wrapping my head around this.</t>
+  </si>
+  <si>
+    <t>Pay close attention to the process and document it to try and make it make sense.</t>
+  </si>
+  <si>
+    <t>Deleting the old flats is right because the texures will make them (2) up… right??? Yes this is right delete the old flats</t>
+  </si>
+  <si>
+    <t>use the new columns to show new iterations</t>
+  </si>
+  <si>
+    <t>next time sort wads by date this time leading back to 5.25.19</t>
+  </si>
+  <si>
+    <t>To delete the originals copy all flats into texture folder, cut them back to the flats folder, remove the (2)s from the folder and put them in a sub folder.</t>
+  </si>
+  <si>
+    <t>Use the bulk utility to take off the (2) and don’t forget the space</t>
+  </si>
+  <si>
+    <t>Then cut paste them back into the flats folder overriding the original flats, without deselecting delete the selected flats.</t>
   </si>
 </sst>
 </file>
@@ -1310,1236 +1547,1952 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F156"/>
+  <dimension ref="A1:G186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="D155" sqref="D155"/>
+    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
+      <selection activeCell="G166" sqref="G166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
+      <c r="C16" t="s">
+        <v>296</v>
+      </c>
+      <c r="E16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>155</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C17" t="s">
+        <v>155</v>
+      </c>
+      <c r="E17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>156</v>
       </c>
-      <c r="D18" t="s">
+      <c r="C18" t="s">
+        <v>156</v>
+      </c>
+      <c r="E18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>157</v>
       </c>
-      <c r="D19" t="s">
+      <c r="C19" t="s">
+        <v>157</v>
+      </c>
+      <c r="E19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>158</v>
       </c>
-      <c r="D20" t="s">
+      <c r="C20" t="s">
+        <v>158</v>
+      </c>
+      <c r="E20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>159</v>
       </c>
-      <c r="D21" t="s">
+      <c r="C21" t="s">
+        <v>159</v>
+      </c>
+      <c r="E21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>160</v>
       </c>
-      <c r="D22" t="s">
+      <c r="C22" t="s">
+        <v>160</v>
+      </c>
+      <c r="E22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>161</v>
       </c>
-      <c r="D23" t="s">
+      <c r="C23" t="s">
+        <v>161</v>
+      </c>
+      <c r="E23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>162</v>
       </c>
-      <c r="D24" t="s">
+      <c r="C24" t="s">
+        <v>162</v>
+      </c>
+      <c r="E24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>163</v>
       </c>
-      <c r="D25" t="s">
+      <c r="C25" t="s">
+        <v>163</v>
+      </c>
+      <c r="E25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>164</v>
       </c>
-      <c r="D26" t="s">
+      <c r="C26" t="s">
+        <v>164</v>
+      </c>
+      <c r="E26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>165</v>
       </c>
-      <c r="D27" t="s">
+      <c r="C27" t="s">
+        <v>165</v>
+      </c>
+      <c r="E27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>166</v>
       </c>
-      <c r="D28" t="s">
+      <c r="C28" t="s">
+        <v>166</v>
+      </c>
+      <c r="E28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>167</v>
       </c>
-      <c r="D29" t="s">
+      <c r="C29" t="s">
+        <v>167</v>
+      </c>
+      <c r="E29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>168</v>
       </c>
-      <c r="D30" t="s">
+      <c r="C30" t="s">
+        <v>168</v>
+      </c>
+      <c r="E30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>169</v>
       </c>
-      <c r="D31" t="s">
+      <c r="C31" t="s">
+        <v>169</v>
+      </c>
+      <c r="E31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>170</v>
       </c>
-      <c r="D32" t="s">
+      <c r="C32" t="s">
+        <v>170</v>
+      </c>
+      <c r="E32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>171</v>
       </c>
-      <c r="D33" t="s">
+      <c r="C33" t="s">
+        <v>171</v>
+      </c>
+      <c r="E33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>172</v>
       </c>
-      <c r="D34" t="s">
+      <c r="C34" t="s">
+        <v>172</v>
+      </c>
+      <c r="E34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>173</v>
       </c>
-      <c r="D35" t="s">
+      <c r="C35" t="s">
+        <v>173</v>
+      </c>
+      <c r="E35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>174</v>
       </c>
-      <c r="D36" t="s">
+      <c r="C36" t="s">
+        <v>174</v>
+      </c>
+      <c r="E36" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>175</v>
       </c>
-      <c r="D37" t="s">
+      <c r="C37" t="s">
+        <v>175</v>
+      </c>
+      <c r="E37" t="s">
         <v>36</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>176</v>
       </c>
-      <c r="D38" t="s">
+      <c r="C38" t="s">
+        <v>176</v>
+      </c>
+      <c r="E38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>177</v>
       </c>
-      <c r="D39" t="s">
+      <c r="C39" t="s">
+        <v>177</v>
+      </c>
+      <c r="E39" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>178</v>
       </c>
-      <c r="D40" t="s">
+      <c r="C40" t="s">
+        <v>178</v>
+      </c>
+      <c r="E40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>179</v>
       </c>
-      <c r="D41" t="s">
+      <c r="C41" t="s">
+        <v>179</v>
+      </c>
+      <c r="E41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>180</v>
       </c>
-      <c r="D42" t="s">
+      <c r="C42" t="s">
+        <v>180</v>
+      </c>
+      <c r="E42" t="s">
         <v>41</v>
       </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>181</v>
       </c>
-      <c r="D43" t="s">
+      <c r="C43" t="s">
+        <v>181</v>
+      </c>
+      <c r="E43" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>182</v>
       </c>
-      <c r="D44" t="s">
+      <c r="C44" t="s">
+        <v>182</v>
+      </c>
+      <c r="E44" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>183</v>
       </c>
-      <c r="D45" t="s">
+      <c r="C45" t="s">
+        <v>183</v>
+      </c>
+      <c r="E45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>184</v>
       </c>
-      <c r="D46" t="s">
+      <c r="C46" t="s">
+        <v>184</v>
+      </c>
+      <c r="E46" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>185</v>
       </c>
-      <c r="D47" t="s">
+      <c r="C47" t="s">
+        <v>185</v>
+      </c>
+      <c r="E47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>186</v>
       </c>
-      <c r="D48" t="s">
+      <c r="C48" t="s">
+        <v>186</v>
+      </c>
+      <c r="E48" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>187</v>
       </c>
-      <c r="D49" t="s">
+      <c r="C49" t="s">
+        <v>187</v>
+      </c>
+      <c r="E49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>188</v>
       </c>
-      <c r="D50" t="s">
+      <c r="C50" t="s">
+        <v>188</v>
+      </c>
+      <c r="E50" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>189</v>
       </c>
-      <c r="D51" t="s">
+      <c r="C51" t="s">
+        <v>189</v>
+      </c>
+      <c r="E51" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>190</v>
       </c>
-      <c r="D52" t="s">
+      <c r="C52" t="s">
+        <v>190</v>
+      </c>
+      <c r="E52" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>191</v>
       </c>
-      <c r="D53" t="s">
+      <c r="C53" t="s">
+        <v>191</v>
+      </c>
+      <c r="E53" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>192</v>
       </c>
-      <c r="D54" t="s">
+      <c r="C54" t="s">
+        <v>192</v>
+      </c>
+      <c r="E54" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>193</v>
       </c>
-      <c r="D55" t="s">
+      <c r="C55" t="s">
+        <v>193</v>
+      </c>
+      <c r="E55" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>194</v>
       </c>
-      <c r="D56" t="s">
+      <c r="C56" t="s">
+        <v>194</v>
+      </c>
+      <c r="E56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>195</v>
       </c>
-      <c r="D57" t="s">
+      <c r="C57" t="s">
+        <v>195</v>
+      </c>
+      <c r="E57" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>196</v>
       </c>
-      <c r="D58" t="s">
+      <c r="C58" t="s">
+        <v>196</v>
+      </c>
+      <c r="E58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>197</v>
       </c>
-      <c r="D59" t="s">
+      <c r="C59" t="s">
+        <v>197</v>
+      </c>
+      <c r="E59" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>198</v>
       </c>
-      <c r="D60" t="s">
+      <c r="C60" t="s">
+        <v>198</v>
+      </c>
+      <c r="E60" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>199</v>
       </c>
-      <c r="D61" t="s">
+      <c r="C61" t="s">
+        <v>199</v>
+      </c>
+      <c r="E61" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>200</v>
       </c>
-      <c r="D62" t="s">
+      <c r="C62" t="s">
+        <v>200</v>
+      </c>
+      <c r="E62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>201</v>
       </c>
-      <c r="D63" t="s">
+      <c r="C63" t="s">
+        <v>201</v>
+      </c>
+      <c r="E63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>202</v>
       </c>
-      <c r="D64" t="s">
+      <c r="C64" t="s">
+        <v>202</v>
+      </c>
+      <c r="E64" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>203</v>
       </c>
-      <c r="D65" t="s">
+      <c r="C65" t="s">
+        <v>203</v>
+      </c>
+      <c r="E65" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>204</v>
       </c>
-      <c r="D66" t="s">
+      <c r="C66" t="s">
+        <v>204</v>
+      </c>
+      <c r="E66" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>205</v>
       </c>
-      <c r="D67" t="s">
+      <c r="C67" t="s">
+        <v>205</v>
+      </c>
+      <c r="E67" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>206</v>
       </c>
-      <c r="D68" t="s">
+      <c r="C68" t="s">
+        <v>206</v>
+      </c>
+      <c r="E68" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>207</v>
       </c>
-      <c r="D69" t="s">
+      <c r="C69" t="s">
+        <v>207</v>
+      </c>
+      <c r="E69" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>208</v>
       </c>
-      <c r="D70" t="s">
+      <c r="C70" t="s">
+        <v>208</v>
+      </c>
+      <c r="E70" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>209</v>
       </c>
-      <c r="D71" t="s">
+      <c r="C71" t="s">
+        <v>209</v>
+      </c>
+      <c r="E71" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>210</v>
       </c>
-      <c r="D72" t="s">
+      <c r="C72" t="s">
+        <v>210</v>
+      </c>
+      <c r="E72" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>211</v>
       </c>
-      <c r="D73" t="s">
+      <c r="C73" t="s">
+        <v>211</v>
+      </c>
+      <c r="E73" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>212</v>
       </c>
-      <c r="D74" t="s">
+      <c r="C74" t="s">
+        <v>212</v>
+      </c>
+      <c r="E74" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>213</v>
       </c>
-      <c r="D75" t="s">
+      <c r="C75" t="s">
+        <v>213</v>
+      </c>
+      <c r="E75" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>214</v>
       </c>
-      <c r="D76" t="s">
+      <c r="C76" t="s">
+        <v>214</v>
+      </c>
+      <c r="E76" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>215</v>
       </c>
-      <c r="D77" t="s">
+      <c r="C77" t="s">
+        <v>215</v>
+      </c>
+      <c r="E77" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>216</v>
       </c>
-      <c r="D78" t="s">
+      <c r="C78" t="s">
+        <v>216</v>
+      </c>
+      <c r="E78" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>217</v>
       </c>
-      <c r="D79" t="s">
+      <c r="C79" t="s">
+        <v>217</v>
+      </c>
+      <c r="E79" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>218</v>
       </c>
-      <c r="D80" t="s">
+      <c r="C80" t="s">
+        <v>218</v>
+      </c>
+      <c r="E80" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>219</v>
       </c>
-      <c r="D81" t="s">
+      <c r="C81" t="s">
+        <v>219</v>
+      </c>
+      <c r="E81" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>220</v>
       </c>
-      <c r="D82" t="s">
+      <c r="C82" t="s">
+        <v>220</v>
+      </c>
+      <c r="E82" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>221</v>
       </c>
-      <c r="D83" t="s">
+      <c r="C83" t="s">
+        <v>221</v>
+      </c>
+      <c r="E83" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>222</v>
       </c>
-      <c r="D84" t="s">
+      <c r="C84" t="s">
+        <v>222</v>
+      </c>
+      <c r="E84" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>223</v>
       </c>
-      <c r="D85" t="s">
+      <c r="C85" t="s">
+        <v>223</v>
+      </c>
+      <c r="E85" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>224</v>
       </c>
-      <c r="D86" t="s">
+      <c r="C86" t="s">
+        <v>224</v>
+      </c>
+      <c r="E86" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>225</v>
       </c>
-      <c r="D87" t="s">
+      <c r="C87" t="s">
+        <v>225</v>
+      </c>
+      <c r="E87" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>226</v>
       </c>
-      <c r="D88" t="s">
+      <c r="C88" t="s">
+        <v>226</v>
+      </c>
+      <c r="E88" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>227</v>
       </c>
-      <c r="D89" t="s">
+      <c r="C89" t="s">
+        <v>227</v>
+      </c>
+      <c r="E89" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>228</v>
       </c>
-      <c r="D90" t="s">
+      <c r="C90" t="s">
+        <v>228</v>
+      </c>
+      <c r="E90" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>229</v>
       </c>
-      <c r="D91" t="s">
+      <c r="C91" t="s">
+        <v>229</v>
+      </c>
+      <c r="E91" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>230</v>
       </c>
-      <c r="D92" t="s">
+      <c r="C92" t="s">
+        <v>230</v>
+      </c>
+      <c r="E92" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>231</v>
       </c>
-      <c r="D93" t="s">
+      <c r="C93" t="s">
+        <v>231</v>
+      </c>
+      <c r="E93" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>232</v>
       </c>
-      <c r="D94" t="s">
+      <c r="C94" t="s">
+        <v>232</v>
+      </c>
+      <c r="E94" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>233</v>
       </c>
-      <c r="D95" t="s">
+      <c r="C95" t="s">
+        <v>233</v>
+      </c>
+      <c r="E95" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>234</v>
       </c>
-      <c r="D96" t="s">
+      <c r="C96" t="s">
+        <v>234</v>
+      </c>
+      <c r="E96" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>235</v>
       </c>
-      <c r="D97" t="s">
+      <c r="C97" t="s">
+        <v>235</v>
+      </c>
+      <c r="E97" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>236</v>
       </c>
-      <c r="D98" t="s">
+      <c r="C98" t="s">
+        <v>236</v>
+      </c>
+      <c r="E98" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F98" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>237</v>
       </c>
-      <c r="D99" t="s">
+      <c r="C99" t="s">
+        <v>237</v>
+      </c>
+      <c r="E99" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F99" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>238</v>
       </c>
-      <c r="D100" t="s">
+      <c r="C100" t="s">
+        <v>238</v>
+      </c>
+      <c r="E100" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F100" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>239</v>
       </c>
-      <c r="D101" t="s">
+      <c r="C101" t="s">
+        <v>239</v>
+      </c>
+      <c r="E101" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F101" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>240</v>
       </c>
-      <c r="D102" t="s">
+      <c r="C102" t="s">
+        <v>240</v>
+      </c>
+      <c r="E102" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F102" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>241</v>
       </c>
-      <c r="D103" t="s">
+      <c r="C103" t="s">
+        <v>241</v>
+      </c>
+      <c r="E103" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F103" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>242</v>
       </c>
-      <c r="D104" t="s">
+      <c r="C104" t="s">
+        <v>242</v>
+      </c>
+      <c r="E104" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>243</v>
       </c>
-      <c r="D105" t="s">
+      <c r="C105" t="s">
+        <v>243</v>
+      </c>
+      <c r="E105" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F105" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>244</v>
       </c>
-      <c r="D106" t="s">
+      <c r="C106" t="s">
+        <v>244</v>
+      </c>
+      <c r="E106" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>245</v>
       </c>
-      <c r="D107" t="s">
+      <c r="C107" t="s">
+        <v>245</v>
+      </c>
+      <c r="E107" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F107" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>246</v>
       </c>
-      <c r="D108" t="s">
+      <c r="C108" t="s">
+        <v>246</v>
+      </c>
+      <c r="E108" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>247</v>
       </c>
-      <c r="D109" t="s">
+      <c r="C109" t="s">
+        <v>247</v>
+      </c>
+      <c r="E109" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F109" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>248</v>
       </c>
-      <c r="D110" t="s">
+      <c r="C110" t="s">
+        <v>248</v>
+      </c>
+      <c r="E110" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F110" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>249</v>
       </c>
-      <c r="D111" t="s">
+      <c r="C111" t="s">
+        <v>249</v>
+      </c>
+      <c r="E111" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F111" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>250</v>
       </c>
-      <c r="D112" t="s">
+      <c r="C112" t="s">
+        <v>250</v>
+      </c>
+      <c r="E112" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>251</v>
       </c>
-      <c r="D113" t="s">
+      <c r="C113" t="s">
+        <v>251</v>
+      </c>
+      <c r="E113" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F113" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>252</v>
       </c>
-      <c r="D114" t="s">
+      <c r="C114" t="s">
+        <v>252</v>
+      </c>
+      <c r="E114" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>253</v>
       </c>
-      <c r="D115" t="s">
+      <c r="C115" t="s">
+        <v>253</v>
+      </c>
+      <c r="E115" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>254</v>
       </c>
-      <c r="D116" t="s">
+      <c r="C116" t="s">
+        <v>254</v>
+      </c>
+      <c r="E116" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>255</v>
       </c>
-      <c r="D117" t="s">
+      <c r="C117" t="s">
+        <v>255</v>
+      </c>
+      <c r="E117" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>256</v>
       </c>
-      <c r="D118" t="s">
+      <c r="C118" t="s">
+        <v>256</v>
+      </c>
+      <c r="E118" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>257</v>
       </c>
-      <c r="D119" t="s">
+      <c r="C119" t="s">
+        <v>257</v>
+      </c>
+      <c r="E119" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>258</v>
       </c>
-      <c r="D120" t="s">
+      <c r="C120" t="s">
+        <v>258</v>
+      </c>
+      <c r="E120" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>259</v>
       </c>
-      <c r="D121" t="s">
+      <c r="C121" t="s">
+        <v>259</v>
+      </c>
+      <c r="E121" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>260</v>
       </c>
-      <c r="D122" t="s">
+      <c r="C122" t="s">
+        <v>260</v>
+      </c>
+      <c r="E122" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>261</v>
       </c>
-      <c r="D123" t="s">
+      <c r="C123" t="s">
+        <v>261</v>
+      </c>
+      <c r="E123" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>262</v>
       </c>
-      <c r="D124" t="s">
+      <c r="C124" t="s">
+        <v>262</v>
+      </c>
+      <c r="E124" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>263</v>
       </c>
-      <c r="D125" t="s">
+      <c r="C125" t="s">
+        <v>263</v>
+      </c>
+      <c r="E125" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>264</v>
       </c>
-      <c r="D126" t="s">
+      <c r="C126" t="s">
+        <v>264</v>
+      </c>
+      <c r="E126" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>265</v>
       </c>
-      <c r="D127" t="s">
+      <c r="C127" t="s">
+        <v>265</v>
+      </c>
+      <c r="E127" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>266</v>
       </c>
-      <c r="D128" t="s">
+      <c r="C128" t="s">
+        <v>266</v>
+      </c>
+      <c r="E128" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>267</v>
       </c>
-      <c r="D129" t="s">
+      <c r="C129" t="s">
+        <v>267</v>
+      </c>
+      <c r="E129" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>268</v>
       </c>
-      <c r="D130" t="s">
+      <c r="C130" t="s">
+        <v>268</v>
+      </c>
+      <c r="E130" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>269</v>
       </c>
-      <c r="D131" t="s">
+      <c r="C131" t="s">
+        <v>269</v>
+      </c>
+      <c r="E131" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>270</v>
       </c>
-      <c r="D132" t="s">
+      <c r="C132" t="s">
+        <v>270</v>
+      </c>
+      <c r="E132" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>271</v>
       </c>
-      <c r="D133" t="s">
+      <c r="C133" t="s">
+        <v>271</v>
+      </c>
+      <c r="E133" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>272</v>
       </c>
-      <c r="D134" t="s">
+      <c r="C134" t="s">
+        <v>272</v>
+      </c>
+      <c r="E134" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>273</v>
       </c>
-      <c r="D135" t="s">
+      <c r="C135" t="s">
+        <v>273</v>
+      </c>
+      <c r="E135" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>274</v>
       </c>
-      <c r="D136" t="s">
+      <c r="C136" t="s">
+        <v>274</v>
+      </c>
+      <c r="E136" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>275</v>
       </c>
-      <c r="D137" t="s">
+      <c r="C137" t="s">
+        <v>275</v>
+      </c>
+      <c r="E137" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>276</v>
       </c>
-      <c r="D138" t="s">
+      <c r="C138" t="s">
+        <v>276</v>
+      </c>
+      <c r="E138" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>277</v>
       </c>
-      <c r="D139" t="s">
+      <c r="C139" t="s">
+        <v>277</v>
+      </c>
+      <c r="E139" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>278</v>
       </c>
-      <c r="D140" t="s">
+      <c r="C140" t="s">
+        <v>278</v>
+      </c>
+      <c r="E140" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>279</v>
       </c>
-      <c r="D141" t="s">
+      <c r="C141" t="s">
+        <v>279</v>
+      </c>
+      <c r="E141" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>280</v>
       </c>
-      <c r="D142" t="s">
+      <c r="C142" t="s">
+        <v>280</v>
+      </c>
+      <c r="E142" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>281</v>
       </c>
-      <c r="D143" t="s">
+      <c r="C143" t="s">
+        <v>281</v>
+      </c>
+      <c r="E143" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>282</v>
       </c>
-      <c r="D144" t="s">
+      <c r="C144" t="s">
+        <v>282</v>
+      </c>
+      <c r="E144" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>283</v>
       </c>
-      <c r="D145" t="s">
+      <c r="C145" t="s">
+        <v>283</v>
+      </c>
+      <c r="E145" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>284</v>
       </c>
-      <c r="D146" t="s">
+      <c r="C146" t="s">
+        <v>284</v>
+      </c>
+      <c r="E146" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
         <v>285</v>
       </c>
-      <c r="D147" t="s">
+      <c r="C147" t="s">
+        <v>285</v>
+      </c>
+      <c r="E147" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>286</v>
       </c>
-      <c r="D148" t="s">
+      <c r="C148" t="s">
+        <v>286</v>
+      </c>
+      <c r="E148" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>287</v>
       </c>
-      <c r="D149" t="s">
+      <c r="C149" t="s">
+        <v>287</v>
+      </c>
+      <c r="E149" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>288</v>
       </c>
-      <c r="D150" t="s">
+      <c r="C150" t="s">
+        <v>288</v>
+      </c>
+      <c r="E150" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>289</v>
       </c>
-      <c r="D151" t="s">
+      <c r="C151" t="s">
+        <v>289</v>
+      </c>
+      <c r="E151" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>290</v>
       </c>
-      <c r="D152" t="s">
+      <c r="C152" t="s">
+        <v>290</v>
+      </c>
+      <c r="E152" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>291</v>
       </c>
-      <c r="D153" t="s">
+      <c r="C153" t="s">
+        <v>291</v>
+      </c>
+      <c r="E153" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>292</v>
       </c>
-      <c r="D154" t="s">
+      <c r="C154" t="s">
+        <v>292</v>
+      </c>
+      <c r="E154" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>293</v>
       </c>
-      <c r="D155" t="s">
+      <c r="C155" t="s">
+        <v>293</v>
+      </c>
+      <c r="E155" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>2</v>
       </c>
-      <c r="D156" t="s">
-        <v>2</v>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C157" t="s">
+        <v>297</v>
+      </c>
+      <c r="E157" t="s">
+        <v>327</v>
+      </c>
+      <c r="G157" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C158" t="s">
+        <v>298</v>
+      </c>
+      <c r="E158" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C159" t="s">
+        <v>299</v>
+      </c>
+      <c r="E159" t="s">
+        <v>329</v>
+      </c>
+      <c r="G159" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C160" t="s">
+        <v>300</v>
+      </c>
+      <c r="E160" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="161" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C161" t="s">
+        <v>301</v>
+      </c>
+      <c r="E161" t="s">
+        <v>331</v>
+      </c>
+      <c r="G161" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="162" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C162" t="s">
+        <v>302</v>
+      </c>
+      <c r="E162" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="163" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C163" t="s">
+        <v>303</v>
+      </c>
+      <c r="E163" t="s">
+        <v>333</v>
+      </c>
+      <c r="G163" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="164" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C164" t="s">
+        <v>304</v>
+      </c>
+      <c r="E164" t="s">
+        <v>334</v>
+      </c>
+      <c r="G164" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="165" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C165" t="s">
+        <v>305</v>
+      </c>
+      <c r="E165" t="s">
+        <v>335</v>
+      </c>
+      <c r="G165" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="166" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C166" t="s">
+        <v>306</v>
+      </c>
+      <c r="E166" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="167" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C167" t="s">
+        <v>307</v>
+      </c>
+      <c r="E167" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="168" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C168" t="s">
+        <v>308</v>
+      </c>
+      <c r="E168" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="169" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C169" t="s">
+        <v>309</v>
+      </c>
+      <c r="E169" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="170" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C170" t="s">
+        <v>310</v>
+      </c>
+      <c r="E170" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="171" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C171" t="s">
+        <v>311</v>
+      </c>
+      <c r="E171" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="172" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C172" t="s">
+        <v>312</v>
+      </c>
+      <c r="E172" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="173" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C173" t="s">
+        <v>313</v>
+      </c>
+      <c r="E173" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="174" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C174" t="s">
+        <v>314</v>
+      </c>
+      <c r="E174" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="175" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C175" t="s">
+        <v>315</v>
+      </c>
+      <c r="E175" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="176" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C176" t="s">
+        <v>316</v>
+      </c>
+      <c r="E176" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="177" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C177" t="s">
+        <v>317</v>
+      </c>
+      <c r="E177" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="178" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C178" t="s">
+        <v>318</v>
+      </c>
+      <c r="E178" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="179" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C179" t="s">
+        <v>319</v>
+      </c>
+      <c r="E179" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="180" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C180" t="s">
+        <v>320</v>
+      </c>
+      <c r="E180" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="181" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C181" t="s">
+        <v>321</v>
+      </c>
+      <c r="E181" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="182" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C182" t="s">
+        <v>322</v>
+      </c>
+      <c r="E182" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="183" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C183" t="s">
+        <v>323</v>
+      </c>
+      <c r="E183" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="184" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C184" t="s">
+        <v>324</v>
+      </c>
+      <c r="E184" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="185" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C185" t="s">
+        <v>325</v>
+      </c>
+      <c r="E185" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="186" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C186" t="s">
+        <v>326</v>
+      </c>
+      <c r="E186" t="s">
+        <v>356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Zone 300. Ignore bad flats until pre-release
</commit_message>
<xml_diff>
--- a/pk3/FLAT DISAMBIUATOR.xlsx
+++ b/pk3/FLAT DISAMBIUATOR.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="525">
   <si>
     <t>Name</t>
   </si>
@@ -1141,6 +1141,456 @@
   </si>
   <si>
     <t>Then cut paste them back into the flats folder overriding the original flats, without deselecting delete the selected flats.</t>
+  </si>
+  <si>
+    <t>C:\Users\TwoIsOne\Desktop\5.22.19\WORKSPACE8\BAK\D2Flats\</t>
+  </si>
+  <si>
+    <t>BLOOD1.png</t>
+  </si>
+  <si>
+    <t>BLOOD2.png</t>
+  </si>
+  <si>
+    <t>BLOOD3.png</t>
+  </si>
+  <si>
+    <t>CEIL1_1.png</t>
+  </si>
+  <si>
+    <t>CEIL1_2.png</t>
+  </si>
+  <si>
+    <t>CEIL1_3.png</t>
+  </si>
+  <si>
+    <t>CEIL3_1.png</t>
+  </si>
+  <si>
+    <t>CEIL3_2.png</t>
+  </si>
+  <si>
+    <t>CEIL3_3.png</t>
+  </si>
+  <si>
+    <t>CEIL3_4.png</t>
+  </si>
+  <si>
+    <t>CEIL3_5.png</t>
+  </si>
+  <si>
+    <t>CEIL3_6.png</t>
+  </si>
+  <si>
+    <t>CEIL4_1.png</t>
+  </si>
+  <si>
+    <t>CEIL4_2.png</t>
+  </si>
+  <si>
+    <t>CEIL4_3.png</t>
+  </si>
+  <si>
+    <t>CEIL5_1.png</t>
+  </si>
+  <si>
+    <t>CEIL5_2.png</t>
+  </si>
+  <si>
+    <t>COMP01.png</t>
+  </si>
+  <si>
+    <t>CONS1_1.png</t>
+  </si>
+  <si>
+    <t>CONS1_5.png</t>
+  </si>
+  <si>
+    <t>CONS1_7.png</t>
+  </si>
+  <si>
+    <t>CRATOP1.png</t>
+  </si>
+  <si>
+    <t>CRATOP2.png</t>
+  </si>
+  <si>
+    <t>DEM1_1.png</t>
+  </si>
+  <si>
+    <t>DEM1_2.png</t>
+  </si>
+  <si>
+    <t>DEM1_3.png</t>
+  </si>
+  <si>
+    <t>DEM1_4.png</t>
+  </si>
+  <si>
+    <t>DEM1_5.png</t>
+  </si>
+  <si>
+    <t>DEM1_6.png</t>
+  </si>
+  <si>
+    <t>F_SKY1.png</t>
+  </si>
+  <si>
+    <t>FLAT1.png</t>
+  </si>
+  <si>
+    <t>FLAT1_1.png</t>
+  </si>
+  <si>
+    <t>FLAT1_2.png</t>
+  </si>
+  <si>
+    <t>FLAT1_3.png</t>
+  </si>
+  <si>
+    <t>FLAT2.png</t>
+  </si>
+  <si>
+    <t>FLAT3.png</t>
+  </si>
+  <si>
+    <t>FLAT4.png</t>
+  </si>
+  <si>
+    <t>FLAT5.png</t>
+  </si>
+  <si>
+    <t>FLAT5_1.png</t>
+  </si>
+  <si>
+    <t>FLAT5_2.png</t>
+  </si>
+  <si>
+    <t>FLAT5_3.png</t>
+  </si>
+  <si>
+    <t>FLAT5_4.png</t>
+  </si>
+  <si>
+    <t>FLAT5_5.png</t>
+  </si>
+  <si>
+    <t>FLAT5_6.png</t>
+  </si>
+  <si>
+    <t>FLAT5_7.png</t>
+  </si>
+  <si>
+    <t>FLAT5_8.png</t>
+  </si>
+  <si>
+    <t>FLAT8.png</t>
+  </si>
+  <si>
+    <t>FLAT9.png</t>
+  </si>
+  <si>
+    <t>FLAT10.png</t>
+  </si>
+  <si>
+    <t>FLAT14.png</t>
+  </si>
+  <si>
+    <t>FLAT17.png</t>
+  </si>
+  <si>
+    <t>FLAT18.png</t>
+  </si>
+  <si>
+    <t>FLAT19.png</t>
+  </si>
+  <si>
+    <t>FLAT20.png</t>
+  </si>
+  <si>
+    <t>FLAT22.png</t>
+  </si>
+  <si>
+    <t>FLAT23.png</t>
+  </si>
+  <si>
+    <t>FLOOR0_1.png</t>
+  </si>
+  <si>
+    <t>FLOOR0_2.png</t>
+  </si>
+  <si>
+    <t>FLOOR0_3.png</t>
+  </si>
+  <si>
+    <t>FLOOR0_5.png</t>
+  </si>
+  <si>
+    <t>FLOOR0_6.png</t>
+  </si>
+  <si>
+    <t>FLOOR0_7.png</t>
+  </si>
+  <si>
+    <t>FLOOR1_1.png</t>
+  </si>
+  <si>
+    <t>FLOOR1_6.png</t>
+  </si>
+  <si>
+    <t>FLOOR1_7.png</t>
+  </si>
+  <si>
+    <t>FLOOR3_3.png</t>
+  </si>
+  <si>
+    <t>FLOOR4_1.png</t>
+  </si>
+  <si>
+    <t>FLOOR4_5.png</t>
+  </si>
+  <si>
+    <t>FLOOR4_6.png</t>
+  </si>
+  <si>
+    <t>FLOOR4_8.png</t>
+  </si>
+  <si>
+    <t>FLOOR5_1.png</t>
+  </si>
+  <si>
+    <t>FLOOR5_2.png</t>
+  </si>
+  <si>
+    <t>FLOOR5_3.png</t>
+  </si>
+  <si>
+    <t>FLOOR5_4.png</t>
+  </si>
+  <si>
+    <t>FLOOR6_1.png</t>
+  </si>
+  <si>
+    <t>FLOOR6_2.png</t>
+  </si>
+  <si>
+    <t>FLOOR7_1.png</t>
+  </si>
+  <si>
+    <t>FLOOR7_2.png</t>
+  </si>
+  <si>
+    <t>FWATER1.png</t>
+  </si>
+  <si>
+    <t>FWATER2.png</t>
+  </si>
+  <si>
+    <t>FWATER3.png</t>
+  </si>
+  <si>
+    <t>FWATER4.png</t>
+  </si>
+  <si>
+    <t>GATE1.png</t>
+  </si>
+  <si>
+    <t>GATE2.png</t>
+  </si>
+  <si>
+    <t>GATE3.png</t>
+  </si>
+  <si>
+    <t>GATE4.png</t>
+  </si>
+  <si>
+    <t>GRASS1.png</t>
+  </si>
+  <si>
+    <t>GRASS2.png</t>
+  </si>
+  <si>
+    <t>GRNLITE1.png</t>
+  </si>
+  <si>
+    <t>GRNROCK.png</t>
+  </si>
+  <si>
+    <t>LAVA1.png</t>
+  </si>
+  <si>
+    <t>LAVA2.png</t>
+  </si>
+  <si>
+    <t>LAVA3.png</t>
+  </si>
+  <si>
+    <t>LAVA4.png</t>
+  </si>
+  <si>
+    <t>MFLR8_1.png</t>
+  </si>
+  <si>
+    <t>MFLR8_2.png</t>
+  </si>
+  <si>
+    <t>MFLR8_3.png</t>
+  </si>
+  <si>
+    <t>MFLR8_4.png</t>
+  </si>
+  <si>
+    <t>NUKAGE1.png</t>
+  </si>
+  <si>
+    <t>NUKAGE2.png</t>
+  </si>
+  <si>
+    <t>NUKAGE3.png</t>
+  </si>
+  <si>
+    <t>RROCK01.png</t>
+  </si>
+  <si>
+    <t>RROCK02.png</t>
+  </si>
+  <si>
+    <t>RROCK03.png</t>
+  </si>
+  <si>
+    <t>RROCK04.png</t>
+  </si>
+  <si>
+    <t>RROCK05.png</t>
+  </si>
+  <si>
+    <t>RROCK06.png</t>
+  </si>
+  <si>
+    <t>RROCK07.png</t>
+  </si>
+  <si>
+    <t>RROCK08.png</t>
+  </si>
+  <si>
+    <t>RROCK09.png</t>
+  </si>
+  <si>
+    <t>RROCK10.png</t>
+  </si>
+  <si>
+    <t>RROCK11.png</t>
+  </si>
+  <si>
+    <t>RROCK12.png</t>
+  </si>
+  <si>
+    <t>RROCK13.png</t>
+  </si>
+  <si>
+    <t>RROCK14.png</t>
+  </si>
+  <si>
+    <t>RROCK15.png</t>
+  </si>
+  <si>
+    <t>RROCK16.png</t>
+  </si>
+  <si>
+    <t>RROCK17.png</t>
+  </si>
+  <si>
+    <t>RROCK18.png</t>
+  </si>
+  <si>
+    <t>RROCK19.png</t>
+  </si>
+  <si>
+    <t>RROCK20.png</t>
+  </si>
+  <si>
+    <t>SFLR6_1.png</t>
+  </si>
+  <si>
+    <t>SFLR6_4.png</t>
+  </si>
+  <si>
+    <t>SFLR7_1.png</t>
+  </si>
+  <si>
+    <t>SFLR7_4.png</t>
+  </si>
+  <si>
+    <t>SLIME01.png</t>
+  </si>
+  <si>
+    <t>SLIME02.png</t>
+  </si>
+  <si>
+    <t>SLIME03.png</t>
+  </si>
+  <si>
+    <t>SLIME04.png</t>
+  </si>
+  <si>
+    <t>SLIME05.png</t>
+  </si>
+  <si>
+    <t>SLIME06.png</t>
+  </si>
+  <si>
+    <t>SLIME07.png</t>
+  </si>
+  <si>
+    <t>SLIME08.png</t>
+  </si>
+  <si>
+    <t>SLIME09.png</t>
+  </si>
+  <si>
+    <t>SLIME10.png</t>
+  </si>
+  <si>
+    <t>SLIME11.png</t>
+  </si>
+  <si>
+    <t>SLIME12.png</t>
+  </si>
+  <si>
+    <t>SLIME13.png</t>
+  </si>
+  <si>
+    <t>SLIME14.png</t>
+  </si>
+  <si>
+    <t>SLIME15.png</t>
+  </si>
+  <si>
+    <t>SLIME16.png</t>
+  </si>
+  <si>
+    <t>STEP1.png</t>
+  </si>
+  <si>
+    <t>STEP2.png</t>
+  </si>
+  <si>
+    <t>TLITE6_1.png</t>
+  </si>
+  <si>
+    <t>TLITE6_4.png</t>
+  </si>
+  <si>
+    <t>TLITE6_5.png</t>
+  </si>
+  <si>
+    <t>TLITE6_6.png</t>
+  </si>
+  <si>
+    <t>d2flats</t>
+  </si>
+  <si>
+    <t>some excel magic could help to see what innate flats has been disamiguated, they will be much more common to need replacement in the wads</t>
   </si>
 </sst>
 </file>
@@ -1547,10 +1997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G186"/>
+  <dimension ref="A1:I186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="G166" sqref="G166"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1558,99 +2008,151 @@
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I13" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I14" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -1660,8 +2162,11 @@
       <c r="E16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I16" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>155</v>
       </c>
@@ -1671,8 +2176,11 @@
       <c r="E17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>156</v>
       </c>
@@ -1682,8 +2190,11 @@
       <c r="E18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>157</v>
       </c>
@@ -1693,8 +2204,11 @@
       <c r="E19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>158</v>
       </c>
@@ -1704,8 +2218,11 @@
       <c r="E20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I20" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>159</v>
       </c>
@@ -1715,8 +2232,11 @@
       <c r="E21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I21" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>160</v>
       </c>
@@ -1726,8 +2246,11 @@
       <c r="E22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>161</v>
       </c>
@@ -1737,8 +2260,11 @@
       <c r="E23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>162</v>
       </c>
@@ -1748,8 +2274,11 @@
       <c r="E24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>163</v>
       </c>
@@ -1759,8 +2288,11 @@
       <c r="E25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>164</v>
       </c>
@@ -1770,8 +2302,11 @@
       <c r="E26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>165</v>
       </c>
@@ -1781,8 +2316,11 @@
       <c r="E27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I27" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>166</v>
       </c>
@@ -1792,8 +2330,11 @@
       <c r="E28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I28" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>167</v>
       </c>
@@ -1803,8 +2344,11 @@
       <c r="E29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>168</v>
       </c>
@@ -1814,8 +2358,11 @@
       <c r="E30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I30" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>169</v>
       </c>
@@ -1825,8 +2372,11 @@
       <c r="E31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I31" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>170</v>
       </c>
@@ -1836,8 +2386,11 @@
       <c r="E32" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I32" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>171</v>
       </c>
@@ -1847,8 +2400,11 @@
       <c r="E33" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I33" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>172</v>
       </c>
@@ -1858,8 +2414,11 @@
       <c r="E34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I34" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>173</v>
       </c>
@@ -1869,8 +2428,11 @@
       <c r="E35" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>174</v>
       </c>
@@ -1880,8 +2442,11 @@
       <c r="E36" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>175</v>
       </c>
@@ -1894,8 +2459,11 @@
       <c r="G37" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I37" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>176</v>
       </c>
@@ -1905,8 +2473,11 @@
       <c r="E38" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I38" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>177</v>
       </c>
@@ -1916,8 +2487,11 @@
       <c r="E39" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I39" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>178</v>
       </c>
@@ -1927,8 +2501,11 @@
       <c r="E40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I40" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>179</v>
       </c>
@@ -1938,8 +2515,11 @@
       <c r="E41" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I41" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>180</v>
       </c>
@@ -1952,8 +2532,11 @@
       <c r="F42" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I42" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>181</v>
       </c>
@@ -1963,8 +2546,11 @@
       <c r="E43" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>182</v>
       </c>
@@ -1974,8 +2560,11 @@
       <c r="E44" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I44" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>183</v>
       </c>
@@ -1985,8 +2574,11 @@
       <c r="E45" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>184</v>
       </c>
@@ -1996,8 +2588,11 @@
       <c r="E46" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I46" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>185</v>
       </c>
@@ -2007,8 +2602,11 @@
       <c r="E47" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I47" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>186</v>
       </c>
@@ -2018,8 +2616,11 @@
       <c r="E48" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I48" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>187</v>
       </c>
@@ -2029,8 +2630,11 @@
       <c r="E49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I49" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>188</v>
       </c>
@@ -2040,8 +2644,11 @@
       <c r="E50" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I50" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>189</v>
       </c>
@@ -2051,8 +2658,11 @@
       <c r="E51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I51" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>190</v>
       </c>
@@ -2062,8 +2672,11 @@
       <c r="E52" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I52" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>191</v>
       </c>
@@ -2073,8 +2686,11 @@
       <c r="E53" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I53" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>192</v>
       </c>
@@ -2084,8 +2700,11 @@
       <c r="E54" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I54" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>193</v>
       </c>
@@ -2095,8 +2714,11 @@
       <c r="E55" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I55" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>194</v>
       </c>
@@ -2106,8 +2728,11 @@
       <c r="E56" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I56" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>195</v>
       </c>
@@ -2117,8 +2742,11 @@
       <c r="E57" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I57" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>196</v>
       </c>
@@ -2128,8 +2756,11 @@
       <c r="E58" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I58" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>197</v>
       </c>
@@ -2139,8 +2770,11 @@
       <c r="E59" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I59" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>198</v>
       </c>
@@ -2150,8 +2784,11 @@
       <c r="E60" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I60" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>199</v>
       </c>
@@ -2161,8 +2798,11 @@
       <c r="E61" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I61" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>200</v>
       </c>
@@ -2172,8 +2812,11 @@
       <c r="E62" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I62" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>201</v>
       </c>
@@ -2183,8 +2826,11 @@
       <c r="E63" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I63" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>202</v>
       </c>
@@ -2194,8 +2840,11 @@
       <c r="E64" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I64" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>203</v>
       </c>
@@ -2205,8 +2854,11 @@
       <c r="E65" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I65" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>204</v>
       </c>
@@ -2216,8 +2868,11 @@
       <c r="E66" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I66" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>205</v>
       </c>
@@ -2227,8 +2882,11 @@
       <c r="E67" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I67" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>206</v>
       </c>
@@ -2238,8 +2896,11 @@
       <c r="E68" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I68" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>207</v>
       </c>
@@ -2249,8 +2910,11 @@
       <c r="E69" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I69" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>208</v>
       </c>
@@ -2260,8 +2924,11 @@
       <c r="E70" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I70" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>209</v>
       </c>
@@ -2271,8 +2938,11 @@
       <c r="E71" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I71" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>210</v>
       </c>
@@ -2282,8 +2952,11 @@
       <c r="E72" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I72" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>211</v>
       </c>
@@ -2293,8 +2966,11 @@
       <c r="E73" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I73" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>212</v>
       </c>
@@ -2304,8 +2980,11 @@
       <c r="E74" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I74" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>213</v>
       </c>
@@ -2315,8 +2994,11 @@
       <c r="E75" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I75" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>214</v>
       </c>
@@ -2326,8 +3008,11 @@
       <c r="E76" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I76" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>215</v>
       </c>
@@ -2337,8 +3022,11 @@
       <c r="E77" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I77" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>216</v>
       </c>
@@ -2348,8 +3036,11 @@
       <c r="E78" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I78" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>217</v>
       </c>
@@ -2359,8 +3050,11 @@
       <c r="E79" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I79" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>218</v>
       </c>
@@ -2370,8 +3064,11 @@
       <c r="E80" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I80" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>219</v>
       </c>
@@ -2381,8 +3078,11 @@
       <c r="E81" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I81" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>220</v>
       </c>
@@ -2392,8 +3092,11 @@
       <c r="E82" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I82" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>221</v>
       </c>
@@ -2403,8 +3106,11 @@
       <c r="E83" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I83" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>222</v>
       </c>
@@ -2414,8 +3120,11 @@
       <c r="E84" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I84" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>223</v>
       </c>
@@ -2425,8 +3134,11 @@
       <c r="E85" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I85" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>224</v>
       </c>
@@ -2436,8 +3148,11 @@
       <c r="E86" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I86" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>225</v>
       </c>
@@ -2447,8 +3162,11 @@
       <c r="E87" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I87" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>226</v>
       </c>
@@ -2458,8 +3176,11 @@
       <c r="E88" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I88" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="89" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>227</v>
       </c>
@@ -2469,8 +3190,11 @@
       <c r="E89" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I89" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="90" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>228</v>
       </c>
@@ -2480,8 +3204,11 @@
       <c r="E90" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I90" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="91" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>229</v>
       </c>
@@ -2491,8 +3218,11 @@
       <c r="E91" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I91" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="92" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>230</v>
       </c>
@@ -2502,8 +3232,11 @@
       <c r="E92" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I92" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="93" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>231</v>
       </c>
@@ -2513,8 +3246,11 @@
       <c r="E93" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I93" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="94" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>232</v>
       </c>
@@ -2524,8 +3260,11 @@
       <c r="E94" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I94" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="95" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>233</v>
       </c>
@@ -2535,8 +3274,11 @@
       <c r="E95" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I95" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="96" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>234</v>
       </c>
@@ -2546,8 +3288,11 @@
       <c r="E96" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I96" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>235</v>
       </c>
@@ -2557,8 +3302,11 @@
       <c r="E97" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I97" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>236</v>
       </c>
@@ -2571,8 +3319,11 @@
       <c r="F98" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I98" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>237</v>
       </c>
@@ -2585,8 +3336,11 @@
       <c r="F99" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I99" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>238</v>
       </c>
@@ -2599,8 +3353,11 @@
       <c r="F100" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I100" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>239</v>
       </c>
@@ -2613,8 +3370,11 @@
       <c r="F101" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I101" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>240</v>
       </c>
@@ -2627,8 +3387,11 @@
       <c r="F102" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I102" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="103" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>241</v>
       </c>
@@ -2641,8 +3404,11 @@
       <c r="F103" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I103" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>242</v>
       </c>
@@ -2652,8 +3418,11 @@
       <c r="E104" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I104" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>243</v>
       </c>
@@ -2666,8 +3435,11 @@
       <c r="F105" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I105" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>244</v>
       </c>
@@ -2677,8 +3449,11 @@
       <c r="E106" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I106" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>245</v>
       </c>
@@ -2691,8 +3466,11 @@
       <c r="F107" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I107" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>246</v>
       </c>
@@ -2702,8 +3480,11 @@
       <c r="E108" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I108" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>247</v>
       </c>
@@ -2716,8 +3497,11 @@
       <c r="F109" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I109" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>248</v>
       </c>
@@ -2730,8 +3514,11 @@
       <c r="F110" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I110" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>249</v>
       </c>
@@ -2744,8 +3531,11 @@
       <c r="F111" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I111" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
         <v>250</v>
       </c>
@@ -2755,8 +3545,11 @@
       <c r="E112" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I112" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="113" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>251</v>
       </c>
@@ -2769,8 +3562,11 @@
       <c r="F113" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I113" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="114" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>252</v>
       </c>
@@ -2780,8 +3576,11 @@
       <c r="E114" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I114" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="115" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>253</v>
       </c>
@@ -2791,8 +3590,11 @@
       <c r="E115" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I115" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="116" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>254</v>
       </c>
@@ -2802,8 +3604,11 @@
       <c r="E116" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I116" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="117" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>255</v>
       </c>
@@ -2813,8 +3618,11 @@
       <c r="E117" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I117" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="118" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>256</v>
       </c>
@@ -2824,8 +3632,11 @@
       <c r="E118" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I118" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="119" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>257</v>
       </c>
@@ -2835,8 +3646,11 @@
       <c r="E119" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I119" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="120" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>258</v>
       </c>
@@ -2846,8 +3660,11 @@
       <c r="E120" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I120" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="121" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>259</v>
       </c>
@@ -2857,8 +3674,11 @@
       <c r="E121" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I121" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="122" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>260</v>
       </c>
@@ -2868,8 +3688,11 @@
       <c r="E122" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I122" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="123" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>261</v>
       </c>
@@ -2879,8 +3702,11 @@
       <c r="E123" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I123" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="124" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>262</v>
       </c>
@@ -2890,8 +3716,11 @@
       <c r="E124" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I124" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="125" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>263</v>
       </c>
@@ -2901,8 +3730,11 @@
       <c r="E125" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I125" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="126" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>264</v>
       </c>
@@ -2912,8 +3744,11 @@
       <c r="E126" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I126" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="127" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>265</v>
       </c>
@@ -2923,8 +3758,11 @@
       <c r="E127" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I127" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="128" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>266</v>
       </c>
@@ -2934,8 +3772,11 @@
       <c r="E128" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I128" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="129" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>267</v>
       </c>
@@ -2945,8 +3786,11 @@
       <c r="E129" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I129" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="130" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>268</v>
       </c>
@@ -2956,8 +3800,11 @@
       <c r="E130" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I130" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="131" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>269</v>
       </c>
@@ -2967,8 +3814,11 @@
       <c r="E131" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I131" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="132" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>270</v>
       </c>
@@ -2978,8 +3828,11 @@
       <c r="E132" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I132" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="133" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
         <v>271</v>
       </c>
@@ -2989,8 +3842,11 @@
       <c r="E133" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I133" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="134" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>272</v>
       </c>
@@ -3000,8 +3856,11 @@
       <c r="E134" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I134" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="135" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
         <v>273</v>
       </c>
@@ -3011,8 +3870,11 @@
       <c r="E135" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I135" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="136" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
         <v>274</v>
       </c>
@@ -3022,8 +3884,11 @@
       <c r="E136" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I136" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="137" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>275</v>
       </c>
@@ -3033,8 +3898,11 @@
       <c r="E137" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I137" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="138" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
         <v>276</v>
       </c>
@@ -3044,8 +3912,11 @@
       <c r="E138" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I138" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="139" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>277</v>
       </c>
@@ -3055,8 +3926,11 @@
       <c r="E139" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I139" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="140" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
         <v>278</v>
       </c>
@@ -3066,8 +3940,11 @@
       <c r="E140" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I140" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="141" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
         <v>279</v>
       </c>
@@ -3077,8 +3954,11 @@
       <c r="E141" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="142" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I141" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="142" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
         <v>280</v>
       </c>
@@ -3088,8 +3968,11 @@
       <c r="E142" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="143" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I142" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="143" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
         <v>281</v>
       </c>
@@ -3099,8 +3982,11 @@
       <c r="E143" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="144" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="I143" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="144" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>282</v>
       </c>
@@ -3110,8 +3996,11 @@
       <c r="E144" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I144" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>283</v>
       </c>
@@ -3121,8 +4010,11 @@
       <c r="E145" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I145" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
         <v>284</v>
       </c>
@@ -3132,8 +4024,11 @@
       <c r="E146" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I146" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
         <v>285</v>
       </c>
@@ -3143,8 +4038,11 @@
       <c r="E147" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I147" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>286</v>
       </c>
@@ -3154,8 +4052,11 @@
       <c r="E148" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I148" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>287</v>
       </c>
@@ -3165,8 +4066,11 @@
       <c r="E149" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I149" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
         <v>288</v>
       </c>
@@ -3176,8 +4080,11 @@
       <c r="E150" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I150" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
         <v>289</v>
       </c>
@@ -3188,7 +4095,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
         <v>290</v>
       </c>
@@ -3199,7 +4106,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>291</v>
       </c>
@@ -3210,7 +4117,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B154" t="s">
         <v>292</v>
       </c>
@@ -3221,7 +4128,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B155" t="s">
         <v>293</v>
       </c>
@@ -3232,12 +4139,12 @@
         <v>154</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C157" t="s">
         <v>297</v>
       </c>
@@ -3248,7 +4155,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C158" t="s">
         <v>298</v>
       </c>
@@ -3256,7 +4163,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C159" t="s">
         <v>299</v>
       </c>
@@ -3267,7 +4174,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C160" t="s">
         <v>300</v>
       </c>

</xml_diff>